<commit_message>
updated question codes document
</commit_message>
<xml_diff>
--- a/question-codes.xlsx
+++ b/question-codes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arlincherian/pmv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B1FBE29-1F90-CD44-A18A-845B96579316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F3E679-49BA-1445-813F-DEDAA605EAE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8460" yWindow="800" windowWidth="20340" windowHeight="15880" xr2:uid="{2C99850C-D5C6-E141-B89E-DC5E8B547061}"/>
+    <workbookView xWindow="14720" yWindow="860" windowWidth="20340" windowHeight="15880" activeTab="1" xr2:uid="{2C99850C-D5C6-E141-B89E-DC5E8B547061}"/>
   </bookViews>
   <sheets>
     <sheet name="pre-survey" sheetId="1" r:id="rId1"/>
@@ -593,7 +593,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A81AF92-9225-9044-8DD8-45BF73B20332}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -690,13 +690,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E95798C-32DE-D94C-BE45-9EC9FFC0BB3B}">
   <dimension ref="A1:W28"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="39.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.2">

</xml_diff>